<commit_message>
Updated project plan (issue 18) and corrected spelling mistakes in group list
</commit_message>
<xml_diff>
--- a/man/group list.xlsx
+++ b/man/group list.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Github\CS221\man\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="120" yWindow="132" windowWidth="24912" windowHeight="12096"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +47,6 @@
     <t>Project Leader</t>
   </si>
   <si>
-    <t xml:space="preserve">Josh Doyle </t>
-  </si>
-  <si>
     <t>jod32</t>
   </si>
   <si>
@@ -54,9 +56,6 @@
     <t>Deputy QA</t>
   </si>
   <si>
-    <t>Olver Earl</t>
-  </si>
-  <si>
     <t>ole4</t>
   </si>
   <si>
@@ -160,6 +159,12 @@
   </si>
   <si>
     <t>http://users.aber.ac.uk/tma1/wordpress/?feed=rss2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Doyle </t>
+  </si>
+  <si>
+    <t>Oliver Earl</t>
   </si>
 </sst>
 </file>
@@ -234,6 +239,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -281,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,7 +324,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,19 +536,19 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="16.140625" customWidth="1"/>
+    <col min="2" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -554,33 +562,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,124 +602,124 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +746,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -750,7 +758,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added preliminary teams to group list
</commit_message>
<xml_diff>
--- a/man/group list.xlsx
+++ b/man/group list.xlsx
@@ -12,16 +12,16 @@
     <workbookView xWindow="120" yWindow="132" windowWidth="24912" windowHeight="12096"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Group List" sheetId="1" r:id="rId1"/>
+    <sheet name="Java Team" sheetId="2" r:id="rId2"/>
+    <sheet name="Web Team" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Full Name</t>
   </si>
@@ -165,13 +165,91 @@
   </si>
   <si>
     <t>Oliver Earl</t>
+  </si>
+  <si>
+    <t>Stregnth</t>
+  </si>
+  <si>
+    <t>Weakeness</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Web/DB?</t>
+  </si>
+  <si>
+    <t>Lead?</t>
+  </si>
+  <si>
+    <t>Java?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Web?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java </t>
+  </si>
+  <si>
+    <t>Web/DB/Basic Java</t>
+  </si>
+  <si>
+    <t>Java (Rusty) / Web</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Java (y)</t>
+  </si>
+  <si>
+    <t>DB (y) /Web</t>
+  </si>
+  <si>
+    <t>Testing/?</t>
+  </si>
+  <si>
+    <t>Joshua Doyle</t>
+  </si>
+  <si>
+    <t>Team Leader</t>
+  </si>
+  <si>
+    <t>Team Members</t>
+  </si>
+  <si>
+    <t>Ben Dudley?</t>
+  </si>
+  <si>
+    <t>Team Leader?</t>
+  </si>
+  <si>
+    <t>Team member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oliver Earl </t>
+  </si>
+  <si>
+    <t>Team member?</t>
+  </si>
+  <si>
+    <t>Team Members?</t>
+  </si>
+  <si>
+    <t>Web/Small Java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +279,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,11 +308,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -533,22 +619,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
     <col min="5" max="5" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,8 +655,17 @@
       <c r="F1" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -587,8 +684,17 @@
       <c r="F2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -607,8 +713,17 @@
       <c r="F3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -627,8 +742,17 @@
       <c r="F4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -647,8 +771,17 @@
       <c r="F5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -667,8 +800,17 @@
       <c r="F6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -681,8 +823,17 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -701,8 +852,17 @@
       <c r="F8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="G8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -720,6 +880,15 @@
       </c>
       <c r="F9" t="s">
         <v>45</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -742,24 +911,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated group list and fixed spelling mistakes
</commit_message>
<xml_diff>
--- a/man/group list.xlsx
+++ b/man/group list.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Github\CS221\man\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="132" windowWidth="24912" windowHeight="12096"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Group List" sheetId="1" r:id="rId1"/>
     <sheet name="Java Team" sheetId="2" r:id="rId2"/>
     <sheet name="Web Team" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t>Full Name</t>
   </si>
@@ -167,12 +162,6 @@
     <t>Oliver Earl</t>
   </si>
   <si>
-    <t>Stregnth</t>
-  </si>
-  <si>
-    <t>Weakeness</t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
@@ -182,24 +171,12 @@
     <t>Web/DB?</t>
   </si>
   <si>
-    <t>Lead?</t>
-  </si>
-  <si>
     <t>Java?</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Web?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Java </t>
   </si>
   <si>
-    <t>Web/DB/Basic Java</t>
-  </si>
-  <si>
     <t>Java (Rusty) / Web</t>
   </si>
   <si>
@@ -209,12 +186,6 @@
     <t>Java (y)</t>
   </si>
   <si>
-    <t>DB (y) /Web</t>
-  </si>
-  <si>
-    <t>Testing/?</t>
-  </si>
-  <si>
     <t>Joshua Doyle</t>
   </si>
   <si>
@@ -243,6 +214,33 @@
   </si>
   <si>
     <t>Web/Small Java</t>
+  </si>
+  <si>
+    <t>Testing/Web/DB</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Weakness</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>http://mac81cs.blogspot.com/feeds/posts/default</t>
+  </si>
+  <si>
+    <t>http://mac81cs.blogspot.co.uk/</t>
+  </si>
+  <si>
+    <t>Web/Basic Java</t>
+  </si>
+  <si>
+    <t>DB/Basic Java</t>
+  </si>
+  <si>
+    <t>DB (y)</t>
   </si>
 </sst>
 </file>
@@ -375,7 +373,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -621,22 +619,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="23.45" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -656,13 +655,13 @@
         <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -685,13 +684,13 @@
         <v>40</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -714,13 +713,13 @@
         <v>39</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -743,16 +742,16 @@
         <v>41</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -772,13 +771,13 @@
         <v>42</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -801,16 +800,16 @@
         <v>43</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -823,14 +822,20 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -853,13 +858,13 @@
         <v>44</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -882,13 +887,13 @@
         <v>45</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -903,9 +908,10 @@
     <hyperlink ref="E2" r:id="rId5"/>
     <hyperlink ref="E5" r:id="rId6"/>
     <hyperlink ref="E3" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -917,18 +923,18 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -936,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -944,15 +950,15 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -968,18 +974,18 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -987,15 +993,15 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1003,7 +1009,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>